<commit_message>
add sth to design pattern
</commit_message>
<xml_diff>
--- a/实习工作工作投递.xlsx
+++ b/实习工作工作投递.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,15 +92,36 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>未投</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>华硕</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>http://campus.51job.com/asus/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>美团点评</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>后台开发工程师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简历已投</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://campus.meituan.com/#/personal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算法工程师-图像图形
+(实习生)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://campus.alibaba.com/myJobApply.htm?apply=yes&amp;t=1491227550655</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -223,6 +244,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -233,9 +257,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -546,7 +567,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -565,49 +586,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="7"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
@@ -616,9 +637,9 @@
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="8"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" ht="54" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
@@ -639,7 +660,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="4"/>
@@ -664,7 +685,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="J5" s="4"/>
@@ -689,28 +710,34 @@
       <c r="F6" s="4"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="11" t="s">
+      <c r="I6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" ht="27" x14ac:dyDescent="0.15">
       <c r="A7" s="6">
         <v>4</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="6">
+        <v>20170403</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="E7" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
@@ -722,7 +749,7 @@
         <v>20170326</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
@@ -733,8 +760,8 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="11" t="s">
-        <v>21</v>
+      <c r="I8" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="4"/>
@@ -743,14 +770,24 @@
       <c r="A9" s="6">
         <v>6</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="B9" s="3">
+        <v>20170403</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
@@ -922,8 +959,10 @@
     <hyperlink ref="I6" r:id="rId2"/>
     <hyperlink ref="I4" r:id="rId3"/>
     <hyperlink ref="I8" r:id="rId4"/>
+    <hyperlink ref="I9" r:id="rId5" location="/personal"/>
+    <hyperlink ref="I7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>